<commit_message>
Updated crystal caps part numbers in BOM from 0201 to 0603
</commit_message>
<xml_diff>
--- a/RP2040-Breadstick/RaspberryBreadstickBOM.xlsx
+++ b/RP2040-Breadstick/RaspberryBreadstickBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LatteFox\Documents\GitHub\RP2040-Breadstick\RP2040-Breadstick\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990B2819-49E8-4B5F-B117-1B4310317269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B411EA7A-908C-4F3C-A665-5D2C1906D94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{C7BF5387-1B49-4369-B6D8-D04327F8149F}"/>
   </bookViews>
@@ -44,18 +44,6 @@
     <t>Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
-    <t>490-GRM0335C1H100FA01JDKR-ND</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>GRM0335C1H100FA01J</t>
-  </si>
-  <si>
-    <t>81-GRM0335C1H100FA1J</t>
-  </si>
-  <si>
     <t xml:space="preserve">        C202</t>
   </si>
   <si>
@@ -729,19 +717,37 @@
   </si>
   <si>
     <t>0603</t>
+  </si>
+  <si>
+    <t>Walsin Technology Corporation</t>
+  </si>
+  <si>
+    <t>1292-1471-1-ND</t>
+  </si>
+  <si>
+    <t>0603N100J500CT</t>
+  </si>
+  <si>
+    <t>791-0603N100J500CT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -764,9 +770,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,7 +1113,7 @@
   <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,36 +1131,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" t="s">
-        <v>143</v>
-      </c>
       <c r="I1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1162,24 +1169,24 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>228</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>227</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>229</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1188,42 +1195,42 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>228</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>227</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
+        <v>229</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
       </c>
       <c r="I4" s="1">
         <v>1206</v>
@@ -1231,25 +1238,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>13</v>
       </c>
       <c r="I5" s="1">
         <v>1206</v>
@@ -1257,25 +1264,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="H6" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
       </c>
       <c r="I6" s="1">
         <v>1206</v>
@@ -1283,25 +1290,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H7" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
       </c>
       <c r="I7" s="1">
         <v>1206</v>
@@ -1309,25 +1316,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="H8" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
       </c>
       <c r="I8" s="1">
         <v>1206</v>
@@ -1335,25 +1342,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="H9" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
       </c>
       <c r="I9" s="1">
         <v>1206</v>
@@ -1361,77 +1368,77 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="H12" t="s">
         <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
       </c>
       <c r="I12" s="1">
         <v>1206</v>
@@ -1439,25 +1446,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H13" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
       </c>
       <c r="I13" s="1">
         <v>1206</v>
@@ -1465,51 +1472,51 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="G14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="I14" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
         <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" t="s">
-        <v>38</v>
       </c>
       <c r="I15" s="1">
         <v>1206</v>
@@ -1517,1762 +1524,1762 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="B16" t="s">
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
+      <c r="I16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E48" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G49">
         <v>2171790001</v>
       </c>
       <c r="H49" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" t="s">
         <v>55</v>
       </c>
-      <c r="C50" t="s">
+      <c r="I50" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E50" t="s">
-        <v>57</v>
-      </c>
-      <c r="F50" t="s">
-        <v>58</v>
-      </c>
-      <c r="G50" t="s">
-        <v>59</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" t="s">
+        <v>54</v>
+      </c>
+      <c r="G51" t="s">
         <v>55</v>
       </c>
-      <c r="C51" t="s">
+      <c r="I51" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E51" t="s">
-        <v>57</v>
-      </c>
-      <c r="F51" t="s">
-        <v>58</v>
-      </c>
-      <c r="G51" t="s">
-        <v>59</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" t="s">
+        <v>54</v>
+      </c>
+      <c r="G52" t="s">
         <v>55</v>
       </c>
-      <c r="C52" t="s">
+      <c r="I52" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F52" t="s">
-        <v>58</v>
-      </c>
-      <c r="G52" t="s">
-        <v>59</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>54</v>
+      </c>
+      <c r="G53" t="s">
         <v>55</v>
       </c>
-      <c r="C53" t="s">
+      <c r="I53" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E53" t="s">
-        <v>57</v>
-      </c>
-      <c r="F53" t="s">
-        <v>58</v>
-      </c>
-      <c r="G53" t="s">
-        <v>59</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G54" t="s">
         <v>55</v>
       </c>
-      <c r="C54" t="s">
+      <c r="I54" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" t="s">
-        <v>58</v>
-      </c>
-      <c r="G54" t="s">
-        <v>59</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>54</v>
+      </c>
+      <c r="G55" t="s">
         <v>55</v>
       </c>
-      <c r="C55" t="s">
+      <c r="I55" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E55" t="s">
-        <v>57</v>
-      </c>
-      <c r="F55" t="s">
-        <v>58</v>
-      </c>
-      <c r="G55" t="s">
-        <v>59</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B56" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" t="s">
+        <v>54</v>
+      </c>
+      <c r="G56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
+      <c r="I56" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E56" t="s">
-        <v>57</v>
-      </c>
-      <c r="F56" t="s">
-        <v>58</v>
-      </c>
-      <c r="G56" t="s">
-        <v>59</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s">
+        <v>54</v>
+      </c>
+      <c r="G57" t="s">
         <v>55</v>
       </c>
-      <c r="C57" t="s">
+      <c r="I57" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E57" t="s">
-        <v>57</v>
-      </c>
-      <c r="F57" t="s">
-        <v>58</v>
-      </c>
-      <c r="G57" t="s">
-        <v>59</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" t="s">
+        <v>54</v>
+      </c>
+      <c r="G58" t="s">
         <v>55</v>
       </c>
-      <c r="C58" t="s">
+      <c r="I58" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E58" t="s">
-        <v>57</v>
-      </c>
-      <c r="F58" t="s">
-        <v>58</v>
-      </c>
-      <c r="G58" t="s">
-        <v>59</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G59" t="s">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="I59" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E59" t="s">
-        <v>57</v>
-      </c>
-      <c r="F59" t="s">
-        <v>58</v>
-      </c>
-      <c r="G59" t="s">
-        <v>59</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" t="s">
+        <v>53</v>
+      </c>
+      <c r="F60" t="s">
+        <v>54</v>
+      </c>
+      <c r="G60" t="s">
         <v>55</v>
       </c>
-      <c r="C60" t="s">
+      <c r="I60" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E60" t="s">
-        <v>57</v>
-      </c>
-      <c r="F60" t="s">
-        <v>58</v>
-      </c>
-      <c r="G60" t="s">
-        <v>59</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" t="s">
+        <v>54</v>
+      </c>
+      <c r="G61" t="s">
         <v>55</v>
       </c>
-      <c r="C61" t="s">
+      <c r="I61" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E61" t="s">
-        <v>57</v>
-      </c>
-      <c r="F61" t="s">
-        <v>58</v>
-      </c>
-      <c r="G61" t="s">
-        <v>59</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B62" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" t="s">
+        <v>54</v>
+      </c>
+      <c r="G62" t="s">
         <v>55</v>
       </c>
-      <c r="C62" t="s">
+      <c r="I62" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E62" t="s">
-        <v>57</v>
-      </c>
-      <c r="F62" t="s">
-        <v>58</v>
-      </c>
-      <c r="G62" t="s">
-        <v>59</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" t="s">
+        <v>54</v>
+      </c>
+      <c r="G63" t="s">
         <v>55</v>
       </c>
-      <c r="C63" t="s">
+      <c r="I63" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E63" t="s">
-        <v>57</v>
-      </c>
-      <c r="F63" t="s">
-        <v>58</v>
-      </c>
-      <c r="G63" t="s">
-        <v>59</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" t="s">
+        <v>54</v>
+      </c>
+      <c r="G64" t="s">
         <v>55</v>
       </c>
-      <c r="C64" t="s">
+      <c r="I64" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E64" t="s">
-        <v>57</v>
-      </c>
-      <c r="F64" t="s">
-        <v>58</v>
-      </c>
-      <c r="G64" t="s">
-        <v>59</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" t="s">
+        <v>53</v>
+      </c>
+      <c r="F65" t="s">
+        <v>54</v>
+      </c>
+      <c r="G65" t="s">
         <v>55</v>
       </c>
-      <c r="C65" t="s">
+      <c r="I65" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E65" t="s">
-        <v>57</v>
-      </c>
-      <c r="F65" t="s">
-        <v>58</v>
-      </c>
-      <c r="G65" t="s">
-        <v>59</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" t="s">
+        <v>53</v>
+      </c>
+      <c r="F66" t="s">
+        <v>54</v>
+      </c>
+      <c r="G66" t="s">
         <v>55</v>
       </c>
-      <c r="C66" t="s">
+      <c r="I66" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E66" t="s">
-        <v>57</v>
-      </c>
-      <c r="F66" t="s">
-        <v>58</v>
-      </c>
-      <c r="G66" t="s">
-        <v>59</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" t="s">
         <v>55</v>
       </c>
-      <c r="C67" t="s">
+      <c r="I67" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E67" t="s">
-        <v>57</v>
-      </c>
-      <c r="F67" t="s">
-        <v>58</v>
-      </c>
-      <c r="G67" t="s">
-        <v>59</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" t="s">
+        <v>53</v>
+      </c>
+      <c r="F68" t="s">
+        <v>54</v>
+      </c>
+      <c r="G68" t="s">
         <v>55</v>
       </c>
-      <c r="C68" t="s">
+      <c r="I68" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E68" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" t="s">
-        <v>58</v>
-      </c>
-      <c r="G68" t="s">
-        <v>59</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" t="s">
+        <v>53</v>
+      </c>
+      <c r="F69" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69" t="s">
         <v>55</v>
       </c>
-      <c r="C69" t="s">
+      <c r="I69" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E69" t="s">
-        <v>57</v>
-      </c>
-      <c r="F69" t="s">
-        <v>58</v>
-      </c>
-      <c r="G69" t="s">
-        <v>59</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B70" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G70" t="s">
         <v>55</v>
       </c>
-      <c r="C70" t="s">
+      <c r="I70" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E70" t="s">
-        <v>57</v>
-      </c>
-      <c r="F70" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" t="s">
-        <v>59</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" t="s">
+        <v>53</v>
+      </c>
+      <c r="F71" t="s">
+        <v>54</v>
+      </c>
+      <c r="G71" t="s">
         <v>55</v>
       </c>
-      <c r="C71" t="s">
+      <c r="I71" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E71" t="s">
-        <v>57</v>
-      </c>
-      <c r="F71" t="s">
-        <v>58</v>
-      </c>
-      <c r="G71" t="s">
-        <v>59</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" t="s">
+        <v>53</v>
+      </c>
+      <c r="F72" t="s">
+        <v>54</v>
+      </c>
+      <c r="G72" t="s">
         <v>55</v>
       </c>
-      <c r="C72" t="s">
+      <c r="I72" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E72" t="s">
-        <v>57</v>
-      </c>
-      <c r="F72" t="s">
-        <v>58</v>
-      </c>
-      <c r="G72" t="s">
-        <v>59</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" t="s">
+        <v>53</v>
+      </c>
+      <c r="F73" t="s">
+        <v>54</v>
+      </c>
+      <c r="G73" t="s">
         <v>55</v>
       </c>
-      <c r="C73" t="s">
+      <c r="I73" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E73" t="s">
-        <v>57</v>
-      </c>
-      <c r="F73" t="s">
-        <v>58</v>
-      </c>
-      <c r="G73" t="s">
-        <v>59</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" t="s">
+        <v>58</v>
+      </c>
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" t="s">
+        <v>60</v>
+      </c>
+      <c r="G74" t="s">
+        <v>57</v>
+      </c>
+      <c r="H74" t="s">
         <v>61</v>
       </c>
-      <c r="C74" t="s">
+      <c r="I74" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D74" t="s">
-        <v>63</v>
-      </c>
-      <c r="F74" t="s">
-        <v>64</v>
-      </c>
-      <c r="G74" t="s">
-        <v>61</v>
-      </c>
-      <c r="H74" t="s">
-        <v>65</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B75" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75" t="s">
+        <v>60</v>
+      </c>
+      <c r="G75" t="s">
+        <v>57</v>
+      </c>
+      <c r="H75" t="s">
         <v>61</v>
       </c>
-      <c r="C75" t="s">
+      <c r="I75" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D75" t="s">
-        <v>63</v>
-      </c>
-      <c r="F75" t="s">
-        <v>64</v>
-      </c>
-      <c r="G75" t="s">
-        <v>61</v>
-      </c>
-      <c r="H75" t="s">
-        <v>65</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D76" t="s">
+        <v>65</v>
+      </c>
+      <c r="F76" t="s">
+        <v>66</v>
+      </c>
+      <c r="G76" t="s">
         <v>67</v>
       </c>
-      <c r="C76" t="s">
+      <c r="H76" t="s">
         <v>68</v>
       </c>
-      <c r="D76" t="s">
-        <v>69</v>
-      </c>
-      <c r="F76" t="s">
-        <v>70</v>
-      </c>
-      <c r="G76" t="s">
-        <v>71</v>
-      </c>
-      <c r="H76" t="s">
-        <v>72</v>
-      </c>
       <c r="I76" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D77" t="s">
+        <v>65</v>
+      </c>
+      <c r="F77" t="s">
+        <v>66</v>
+      </c>
+      <c r="G77" t="s">
         <v>67</v>
       </c>
-      <c r="C77" t="s">
+      <c r="H77" t="s">
         <v>68</v>
       </c>
-      <c r="D77" t="s">
-        <v>69</v>
-      </c>
-      <c r="F77" t="s">
-        <v>70</v>
-      </c>
-      <c r="G77" t="s">
-        <v>71</v>
-      </c>
-      <c r="H77" t="s">
-        <v>72</v>
-      </c>
       <c r="I77" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" t="s">
+        <v>64</v>
+      </c>
+      <c r="D78" t="s">
+        <v>65</v>
+      </c>
+      <c r="F78" t="s">
+        <v>66</v>
+      </c>
+      <c r="G78" t="s">
         <v>67</v>
       </c>
-      <c r="C78" t="s">
+      <c r="H78" t="s">
         <v>68</v>
       </c>
-      <c r="D78" t="s">
-        <v>69</v>
-      </c>
-      <c r="F78" t="s">
-        <v>70</v>
-      </c>
-      <c r="G78" t="s">
-        <v>71</v>
-      </c>
-      <c r="H78" t="s">
-        <v>72</v>
-      </c>
       <c r="I78" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" t="s">
+        <v>64</v>
+      </c>
+      <c r="D79" t="s">
+        <v>65</v>
+      </c>
+      <c r="F79" t="s">
+        <v>66</v>
+      </c>
+      <c r="G79" t="s">
         <v>67</v>
       </c>
-      <c r="C79" t="s">
+      <c r="H79" t="s">
         <v>68</v>
       </c>
-      <c r="D79" t="s">
-        <v>69</v>
-      </c>
-      <c r="F79" t="s">
-        <v>70</v>
-      </c>
-      <c r="G79" t="s">
-        <v>71</v>
-      </c>
-      <c r="H79" t="s">
-        <v>72</v>
-      </c>
       <c r="I79" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" t="s">
+        <v>64</v>
+      </c>
+      <c r="D80" t="s">
+        <v>65</v>
+      </c>
+      <c r="F80" t="s">
+        <v>66</v>
+      </c>
+      <c r="G80" t="s">
         <v>67</v>
       </c>
-      <c r="C80" t="s">
+      <c r="H80" t="s">
         <v>68</v>
       </c>
-      <c r="D80" t="s">
-        <v>69</v>
-      </c>
-      <c r="F80" t="s">
-        <v>70</v>
-      </c>
-      <c r="G80" t="s">
-        <v>71</v>
-      </c>
-      <c r="H80" t="s">
-        <v>72</v>
-      </c>
       <c r="I80" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B81" t="s">
+        <v>63</v>
+      </c>
+      <c r="C81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" t="s">
+        <v>65</v>
+      </c>
+      <c r="F81" t="s">
+        <v>66</v>
+      </c>
+      <c r="G81" t="s">
         <v>67</v>
       </c>
-      <c r="C81" t="s">
+      <c r="H81" t="s">
         <v>68</v>
       </c>
-      <c r="D81" t="s">
-        <v>69</v>
-      </c>
-      <c r="F81" t="s">
-        <v>70</v>
-      </c>
-      <c r="G81" t="s">
-        <v>71</v>
-      </c>
-      <c r="H81" t="s">
-        <v>72</v>
-      </c>
       <c r="I81" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B82" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82" t="s">
+        <v>64</v>
+      </c>
+      <c r="D82" t="s">
+        <v>65</v>
+      </c>
+      <c r="F82" t="s">
+        <v>66</v>
+      </c>
+      <c r="G82" t="s">
         <v>67</v>
       </c>
-      <c r="C82" t="s">
+      <c r="H82" t="s">
         <v>68</v>
       </c>
-      <c r="D82" t="s">
-        <v>69</v>
-      </c>
-      <c r="F82" t="s">
-        <v>70</v>
-      </c>
-      <c r="G82" t="s">
-        <v>71</v>
-      </c>
-      <c r="H82" t="s">
-        <v>72</v>
-      </c>
       <c r="I82" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B83" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" t="s">
+        <v>64</v>
+      </c>
+      <c r="D83" t="s">
+        <v>65</v>
+      </c>
+      <c r="F83" t="s">
+        <v>66</v>
+      </c>
+      <c r="G83" t="s">
         <v>67</v>
       </c>
-      <c r="C83" t="s">
+      <c r="H83" t="s">
         <v>68</v>
       </c>
-      <c r="D83" t="s">
-        <v>69</v>
-      </c>
-      <c r="F83" t="s">
-        <v>70</v>
-      </c>
-      <c r="G83" t="s">
-        <v>71</v>
-      </c>
-      <c r="H83" t="s">
-        <v>72</v>
-      </c>
       <c r="I83" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D84" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F84" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G84" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H84" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D85" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F85" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G85" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H85" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C86" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D86" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F86" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G86" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H86" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C87" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D87" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F87" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G87" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H87" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C88" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D88" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F88" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G88" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H88" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D89" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F89" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G89" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H89" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90" t="s">
+        <v>74</v>
+      </c>
+      <c r="F90" t="s">
+        <v>66</v>
+      </c>
+      <c r="G90" t="s">
+        <v>75</v>
+      </c>
+      <c r="H90" t="s">
+        <v>76</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B90" t="s">
-        <v>77</v>
-      </c>
-      <c r="C90" t="s">
-        <v>68</v>
-      </c>
-      <c r="D90" t="s">
-        <v>78</v>
-      </c>
-      <c r="F90" t="s">
-        <v>70</v>
-      </c>
-      <c r="G90" t="s">
-        <v>79</v>
-      </c>
-      <c r="H90" t="s">
-        <v>80</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C91" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D91" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F91" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G91" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H91" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C92" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D92" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F92" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G92" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H92" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" t="s">
+        <v>83</v>
+      </c>
+      <c r="D93" t="s">
+        <v>84</v>
+      </c>
+      <c r="F93" t="s">
         <v>85</v>
       </c>
-      <c r="B93" t="s">
+      <c r="G93" t="s">
         <v>86</v>
       </c>
-      <c r="C93" t="s">
+      <c r="H93" t="s">
         <v>87</v>
       </c>
-      <c r="D93" t="s">
+      <c r="I93" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="F93" t="s">
-        <v>89</v>
-      </c>
-      <c r="G93" t="s">
-        <v>90</v>
-      </c>
-      <c r="H93" t="s">
-        <v>91</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C94" t="s">
+        <v>83</v>
+      </c>
+      <c r="D94" t="s">
+        <v>91</v>
+      </c>
+      <c r="F94" t="s">
+        <v>85</v>
+      </c>
+      <c r="G94" t="s">
+        <v>86</v>
+      </c>
+      <c r="H94" t="s">
         <v>87</v>
       </c>
-      <c r="D94" t="s">
-        <v>95</v>
-      </c>
-      <c r="F94" t="s">
-        <v>89</v>
-      </c>
-      <c r="G94" t="s">
-        <v>90</v>
-      </c>
-      <c r="H94" t="s">
-        <v>91</v>
-      </c>
       <c r="I94" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95" t="s">
+        <v>94</v>
+      </c>
+      <c r="D95" t="s">
+        <v>95</v>
+      </c>
+      <c r="E95" t="s">
         <v>96</v>
       </c>
-      <c r="B95" t="s">
+      <c r="F95" t="s">
         <v>97</v>
       </c>
-      <c r="C95" t="s">
+      <c r="G95" t="s">
         <v>98</v>
       </c>
-      <c r="D95" t="s">
+      <c r="H95" t="s">
         <v>99</v>
       </c>
-      <c r="E95" t="s">
+      <c r="I95" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F95" t="s">
-        <v>101</v>
-      </c>
-      <c r="G95" t="s">
-        <v>102</v>
-      </c>
-      <c r="H95" t="s">
-        <v>103</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C96" t="s">
+        <v>103</v>
+      </c>
+      <c r="D96" t="s">
+        <v>104</v>
+      </c>
+      <c r="F96" t="s">
         <v>105</v>
       </c>
-      <c r="B96" t="s">
+      <c r="G96" t="s">
         <v>106</v>
       </c>
-      <c r="C96" t="s">
+      <c r="H96" t="s">
         <v>107</v>
       </c>
-      <c r="D96" t="s">
+      <c r="I96" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F96" t="s">
-        <v>109</v>
-      </c>
-      <c r="G96" t="s">
-        <v>110</v>
-      </c>
-      <c r="H96" t="s">
-        <v>111</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" t="s">
         <v>113</v>
       </c>
-      <c r="B97" t="s">
+      <c r="G97" t="s">
         <v>114</v>
       </c>
-      <c r="C97" t="s">
+      <c r="H97" t="s">
         <v>115</v>
       </c>
-      <c r="D97" t="s">
+      <c r="I97" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F97" t="s">
-        <v>117</v>
-      </c>
-      <c r="G97" t="s">
-        <v>118</v>
-      </c>
-      <c r="H97" t="s">
-        <v>119</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" t="s">
+        <v>119</v>
+      </c>
+      <c r="D98" t="s">
+        <v>120</v>
+      </c>
+      <c r="F98" t="s">
         <v>121</v>
       </c>
-      <c r="B98" t="s">
+      <c r="G98" t="s">
+        <v>118</v>
+      </c>
+      <c r="H98" t="s">
         <v>122</v>
       </c>
-      <c r="C98" t="s">
+      <c r="I98" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D98" t="s">
-        <v>124</v>
-      </c>
-      <c r="F98" t="s">
-        <v>125</v>
-      </c>
-      <c r="G98" t="s">
-        <v>122</v>
-      </c>
-      <c r="H98" t="s">
-        <v>126</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>124</v>
+      </c>
+      <c r="B99" t="s">
+        <v>125</v>
+      </c>
+      <c r="C99" t="s">
+        <v>126</v>
+      </c>
+      <c r="D99" t="s">
+        <v>127</v>
+      </c>
+      <c r="F99" t="s">
         <v>128</v>
       </c>
-      <c r="B99" t="s">
+      <c r="G99" t="s">
         <v>129</v>
       </c>
-      <c r="C99" t="s">
+      <c r="H99" t="s">
         <v>130</v>
       </c>
-      <c r="D99" t="s">
+      <c r="I99" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="F99" t="s">
-        <v>132</v>
-      </c>
-      <c r="G99" t="s">
-        <v>133</v>
-      </c>
-      <c r="H99" t="s">
-        <v>134</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed BOM and Silkscreen
</commit_message>
<xml_diff>
--- a/RP2040-Breadstick/RaspberryBreadstickBOM.xlsx
+++ b/RP2040-Breadstick/RaspberryBreadstickBOM.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LatteFox\Documents\GitHub\RP2040-Breadstick\RP2040-Breadstick\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B411EA7A-908C-4F3C-A665-5D2C1906D94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF3E5B5-0BA3-46FC-BFA4-6D09C3A07FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{C7BF5387-1B49-4369-B6D8-D04327F8149F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PCBWay" sheetId="2" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="263">
   <si>
     <t>10pF 0603</t>
   </si>
@@ -729,13 +730,141 @@
   </si>
   <si>
     <t>791-0603N100J500CT</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>designator</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Qty</t>
+    </r>
+  </si>
+  <si>
+    <t>*Mfg Part #</t>
+  </si>
+  <si>
+    <t>Description / Value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Package</t>
+    </r>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Your Instructions / Notes</t>
+  </si>
+  <si>
+    <t>C204, C206, C302, C304, C306, C402</t>
+  </si>
+  <si>
+    <t>C202, C203</t>
+  </si>
+  <si>
+    <t>C201, C205</t>
+  </si>
+  <si>
+    <t>C501, C502</t>
+  </si>
+  <si>
+    <t>D601</t>
+  </si>
+  <si>
+    <t>F601</t>
+  </si>
+  <si>
+    <t>IC501</t>
+  </si>
+  <si>
+    <t>J601</t>
+  </si>
+  <si>
+    <t>Q301, Q302</t>
+  </si>
+  <si>
+    <t>R201, R203, R301-R304, R501, R502</t>
+  </si>
+  <si>
+    <t>R205, R206</t>
+  </si>
+  <si>
+    <t>R202, R204, R207-R209</t>
+  </si>
+  <si>
+    <t>R601, R602</t>
+  </si>
+  <si>
+    <t>S201</t>
+  </si>
+  <si>
+    <t>S202</t>
+  </si>
+  <si>
+    <t>U201</t>
+  </si>
+  <si>
+    <t>U202</t>
+  </si>
+  <si>
+    <t>U401</t>
+  </si>
+  <si>
+    <t>U501</t>
+  </si>
+  <si>
+    <t>Y201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J101, J102, J103, J104, J105, J106, J107, J108, J109, J110, J111, J112, J113, J114, J115, J116, J117, J118, J119, J120, J121, J122, J123, J124, J125, J126, J127, J128, J129, J130, J131, J132 </t>
+  </si>
+  <si>
+    <t>LED301, LED302, LED303, LED304, LED305, LED306, LED307, LED308, LED309, LED310, LED311, LED312, LED313, LED314, LED315, LED316, LED317, LED318, LED319, LED320, LED321, LED322, LED323, LED324</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>DNP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,16 +878,58 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -766,17 +937,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{5B88A049-46D1-4B05-A7BF-247502A32996}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1109,14 +1314,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C564009-F1E8-49F7-94EA-2FF2F94660B2}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="177.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="62" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2171790001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21" t="s">
+        <v>111</v>
+      </c>
+      <c r="K21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0150D820-641A-4933-98DB-D1FD4F34FFFB}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
@@ -1129,7 +2097,7 @@
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -1158,7 +2126,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1184,7 +2152,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +2178,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1236,7 +2204,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1262,7 +2230,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -1288,7 +2256,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -1314,7 +2282,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -1340,7 +2308,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -1366,7 +2334,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -1392,7 +2360,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -1418,7 +2386,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -1444,7 +2412,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -1470,7 +2438,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1496,7 +2464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1522,7 +2490,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1548,7 +2516,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -1563,7 +2531,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -1578,7 +2546,7 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>152</v>
       </c>
@@ -1593,7 +2561,7 @@
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -1608,7 +2576,7 @@
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -1623,7 +2591,7 @@
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>155</v>
       </c>
@@ -1638,7 +2606,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>156</v>
       </c>
@@ -1653,7 +2621,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>157</v>
       </c>
@@ -1668,7 +2636,7 @@
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -1683,7 +2651,7 @@
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>159</v>
       </c>
@@ -1698,7 +2666,7 @@
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>160</v>
       </c>
@@ -1713,7 +2681,7 @@
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>161</v>
       </c>
@@ -1728,7 +2696,7 @@
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>162</v>
       </c>
@@ -1743,7 +2711,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -1758,7 +2726,7 @@
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -1773,7 +2741,7 @@
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>165</v>
       </c>
@@ -1788,7 +2756,7 @@
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -1803,7 +2771,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>167</v>
       </c>
@@ -1818,7 +2786,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>168</v>
       </c>
@@ -1833,7 +2801,7 @@
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -1848,7 +2816,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>170</v>
       </c>
@@ -1863,7 +2831,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>171</v>
       </c>
@@ -1878,7 +2846,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>172</v>
       </c>
@@ -1893,7 +2861,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -1908,7 +2876,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -1923,7 +2891,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -1938,7 +2906,7 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>176</v>
       </c>
@@ -1953,7 +2921,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>177</v>
       </c>
@@ -1968,7 +2936,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -1983,7 +2951,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>179</v>
       </c>
@@ -1998,7 +2966,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -2013,7 +2981,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>181</v>
       </c>
@@ -2028,7 +2996,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -2051,7 +3019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -2074,7 +3042,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>183</v>
       </c>
@@ -2097,7 +3065,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -2120,7 +3088,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>185</v>
       </c>
@@ -2143,7 +3111,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>186</v>
       </c>
@@ -2166,7 +3134,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>187</v>
       </c>
@@ -2189,7 +3157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>188</v>
       </c>
@@ -2212,7 +3180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -2235,7 +3203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>190</v>
       </c>
@@ -2258,7 +3226,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>191</v>
       </c>
@@ -2281,7 +3249,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>192</v>
       </c>
@@ -2304,7 +3272,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -2327,7 +3295,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>194</v>
       </c>
@@ -2350,7 +3318,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>195</v>
       </c>
@@ -2373,7 +3341,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>196</v>
       </c>
@@ -2396,7 +3364,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -2419,7 +3387,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -2442,7 +3410,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>199</v>
       </c>
@@ -2465,7 +3433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>200</v>
       </c>
@@ -2488,7 +3456,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -2511,7 +3479,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>202</v>
       </c>
@@ -2534,7 +3502,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>203</v>
       </c>
@@ -2557,7 +3525,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>204</v>
       </c>
@@ -2580,7 +3548,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>205</v>
       </c>
@@ -2603,7 +3571,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>206</v>
       </c>
@@ -2629,7 +3597,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>207</v>
       </c>
@@ -2655,7 +3623,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>208</v>
       </c>
@@ -2681,7 +3649,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>209</v>
       </c>
@@ -2707,7 +3675,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>210</v>
       </c>
@@ -2733,7 +3701,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>211</v>
       </c>
@@ -2759,7 +3727,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>212</v>
       </c>
@@ -2785,7 +3753,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>213</v>
       </c>
@@ -2811,7 +3779,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>214</v>
       </c>
@@ -2837,7 +3805,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>215</v>
       </c>
@@ -2863,7 +3831,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>216</v>
       </c>
@@ -2889,7 +3857,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>217</v>
       </c>
@@ -2915,7 +3883,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>218</v>
       </c>
@@ -2941,7 +3909,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>219</v>
       </c>
@@ -2967,7 +3935,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>220</v>
       </c>
@@ -2993,7 +3961,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>221</v>
       </c>
@@ -3019,7 +3987,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>222</v>
       </c>
@@ -3045,7 +4013,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>223</v>
       </c>
@@ -3071,7 +4039,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>224</v>
       </c>
@@ -3097,7 +4065,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>81</v>
       </c>
@@ -3123,7 +4091,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -3149,7 +4117,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -3178,7 +4146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -3204,7 +4172,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -3230,7 +4198,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -3256,7 +4224,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>124</v>
       </c>

</xml_diff>